<commit_message>
updates metadata to match new tables, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-lower-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8A5D29-911B-7849-8559-F6211A07E979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491205C8-CEB9-F640-AE1B-BBAFA988FC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -142,9 +142,6 @@
     <t>whole</t>
   </si>
   <si>
-    <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
-  </si>
-  <si>
     <t>visitTime</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
   </si>
   <si>
     <t>finalRun</t>
-  </si>
-  <si>
-    <t>actualCount</t>
   </si>
   <si>
     <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter").</t>
@@ -521,11 +515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,10 +595,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -715,7 +709,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -791,10 +785,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -870,7 +864,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -923,7 +917,7 @@
         <v>30</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>32</v>
@@ -971,7 +965,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>32</v>
@@ -1019,7 +1013,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>37</v>
@@ -1049,26 +1043,26 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="10">
@@ -1093,10 +1087,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1131,10 +1125,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1169,10 +1163,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1207,10 +1201,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1244,21 +1238,11 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1281,20 +1265,20 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1309,7 +1293,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1321,8 +1305,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1343,14 +1327,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1422,19 +1406,6 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1450,6 +1421,14 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1465,27 +1444,19 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N27" s="4"/>
@@ -1503,19 +1474,19 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N29" s="1"/>
@@ -1533,6 +1504,19 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1632,7 +1616,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -1660,7 +1644,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1688,7 +1672,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1716,7 +1700,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1744,7 +1728,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2696,7 +2680,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
+      <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -28623,50 +28607,22 @@
       <c r="Y997" s="1"/>
       <c r="Z997" s="1"/>
     </row>
-    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="2"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="3"/>
-      <c r="G998" s="3"/>
-      <c r="H998" s="3"/>
-      <c r="I998" s="2"/>
-      <c r="J998" s="3"/>
-      <c r="K998" s="2"/>
-      <c r="L998" s="3"/>
-      <c r="M998" s="3"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C54:C997 C30:C42 C1:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E30:E997 E1:E23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F25 F30:F997 F1:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H25 H30:H997 H1:H23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28693,13 +28649,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28730,10 +28686,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
updates metadata to be consistent across packages
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-lower-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491205C8-CEB9-F640-AE1B-BBAFA988FC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEA5ED0-60B6-3249-807D-327909B54C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,13 +100,7 @@
     <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
-    <t>Common name of species</t>
-  </si>
-  <si>
     <t>fishOrigin</t>
-  </si>
-  <si>
-    <t>Origin/production type of the fish. Levels = c("Hatchery", "Natural", "Unknown")</t>
   </si>
   <si>
     <t>lifeStage</t>
@@ -190,20 +184,10 @@
     <t>finalRun</t>
   </si>
   <si>
-    <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter").</t>
-  </si>
-  <si>
-    <t>Work that was done during visit to trap. Levels = c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", 
-"End trapping")</t>
-  </si>
-  <si>
     <t>Name of the sampling site. Levels = "Lower Feather River RST"</t>
   </si>
   <si>
     <t>Name of the trap or trap location. Levels = c("RL", "RR")</t>
-  </si>
-  <si>
-    <t>Foreign key to the CAMP ProjectDescription table.</t>
   </si>
   <si>
     <t>Lower Feather RST</t>
@@ -212,7 +196,23 @@
     <t>Run designation revised after field visit. This is the field used in analysis. Levels = c("Not recorded", NA, "Spring", "Fall", "Late fall")</t>
   </si>
   <si>
-    <t>Life stage of the fish. Levels = c("Not recorded", "Parr", "Fry", "Juvenile", "Ammocoete", "Yearling", "Silvery parr", "Adult", "YOY (young of the year)", "Yolk sac fry (alevin)", "Smolt")</t>
+    <t>Foreign key to the CAMP ProjectDescription table.  All data associated with this package will have a ProjectDescriptionID = 12.</t>
+  </si>
+  <si>
+    <t>Common name of species. Levels = c("Chinook salmon", "Steelhead / rainbow trout", "Wakasagi / Japanese smelt",  "Inland silverside", "Brown bullhead", "Pacific lamprey", "Sacramento pikeminnow",  "Riffle sculpin", "Channel catfish", "Mosquitofish", "Prickly sculpin",  "Hardhead", "Spotted bass", "Unknown lamprey (Entosphenus or Lampetra)",  "River lamprey", "Common carp", "Tule perch", "Bluegill", "Unknown Centrarchid",  "White crappie", "Black bullhead", "California roach", "Golden shiner",  "Hitch", "Unknown catfish or bullhead", "White catfish", "Smallmouth bass",  "Unknown minnow", "Sacramento sucker", "Warmouth", "Threadfin shad",  "Unknown bass (Micropterus)", "Other", "Largemouth bass", "American shad",  "Goldfish", "Striped bass", "Not yet assigned", "Redear sunfish",  "Green sunfish", "Western brook lamprey", "Red shiner", "Pumpkinseed",  "Black crappie", "Not applicable (n/a)")</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
+  </si>
+  <si>
+    <t>Origin/production type of the fish. Levels =c("Natural", "Hatchery")</t>
+  </si>
+  <si>
+    <t>Life stage of the fish. Levels = c("Not recorded", "Parr", "Fry", "Juvenile", "Ammocoete", "Yearling",  "Silvery parr", "Adult", "YOY (young of the year)", "Yolk sac fry (alevin)" )</t>
+  </si>
+  <si>
+    <t>Work that was done during visit to trap. Levels = c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", 
+"End trapping", "Drive-by only")</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -595,10 +595,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -709,10 +709,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -785,10 +785,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -823,10 +823,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -899,28 +899,28 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
@@ -947,28 +947,28 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
@@ -995,28 +995,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1043,33 +1043,33 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="10">
         <v>44580.520960648151</v>
       </c>
       <c r="M13" s="10">
-        <v>44959.47934027778</v>
+        <v>44991.417326388888</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1125,10 +1125,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -28649,13 +28649,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28686,10 +28686,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
adds visitTime2 on catch and trap as a placeholder
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5589DBA-DCF2-433D-BEF0-86A0EC40BB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F09DB5D-F03E-4A71-AC04-D89710F049F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="650" windowWidth="23200" windowHeight="13420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="2630" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -214,6 +214,12 @@
     <t>Work that was done during visit to trap. Levels = c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", 
 "End trapping", "Drive-by only", "Service/adjust/clean trap")</t>
   </si>
+  <si>
+    <t>visitTime2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
+  </si>
 </sst>
 </file>
 
@@ -274,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -300,6 +306,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1087,48 +1094,50 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1139,14 +1148,14 @@
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1163,10 +1172,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1201,10 +1210,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1238,11 +1247,21 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1265,20 +1284,20 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1293,7 +1312,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1305,8 +1324,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1327,14 +1346,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1406,6 +1425,19 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1421,14 +1453,6 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1444,19 +1468,27 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N27" s="4"/>
@@ -1474,19 +1506,19 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N29" s="1"/>
@@ -1504,19 +1536,6 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1616,7 +1635,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -1644,7 +1663,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1672,7 +1691,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1700,7 +1719,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1728,7 +1747,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2680,7 +2699,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -28607,22 +28626,50 @@
       <c r="Y997" s="1"/>
       <c r="Z997" s="1"/>
     </row>
+    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="3"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="3"/>
+      <c r="M998" s="3"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+      <c r="Z998" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C54:C997 C30:C42 C1:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E30:E997 E1:E23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F25 F30:F997 F1:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H25 H30:H997 H1:H23" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>